<commit_message>
update results and scripts
</commit_message>
<xml_diff>
--- a/swertres/results_filter_excel.xlsx
+++ b/swertres/results_filter_excel.xlsx
@@ -47,52 +47,52 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00775894"/>
+        <fgColor rgb="00773029"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00768037"/>
+        <fgColor rgb="00727845"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00774160"/>
+        <fgColor rgb="00723517"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00768782"/>
+        <fgColor rgb="00721652"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00731341"/>
+        <fgColor rgb="00722606"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00761556"/>
+        <fgColor rgb="00710743"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00769553"/>
+        <fgColor rgb="00705060"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00769982"/>
+        <fgColor rgb="00769800"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00706980"/>
+        <fgColor rgb="00708438"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00729102"/>
+        <fgColor rgb="00721710"/>
       </patternFill>
     </fill>
   </fills>

</xml_diff>